<commit_message>
avance para rendir parcial 2
</commit_message>
<xml_diff>
--- a/gantt-Carrillo_fernando.xlsx
+++ b/gantt-Carrillo_fernando.xlsx
@@ -16,11 +16,12 @@
     <sheet name="Parámetros" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="39">
   <si>
     <t>Abierto</t>
   </si>
@@ -112,23 +113,43 @@
     <t>INICIAR CODIFICACION</t>
   </si>
   <si>
-    <t>TERMIANAR DE CODIFICAR</t>
-  </si>
-  <si>
     <t>EMPEZAR VERIFICACION Y VALIDACION</t>
   </si>
   <si>
     <t>TERMINAR PRUEBAS Y VALIDACIONES</t>
+  </si>
+  <si>
+    <t>Nombre de la tarea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Fecha de inicio</t>
+  </si>
+  <si>
+    <t>Fecha de finalización</t>
+  </si>
+  <si>
+    <t>Asignado</t>
+  </si>
+  <si>
+    <t>Estado</t>
+  </si>
+  <si>
+    <t>TERMINADO</t>
+  </si>
+  <si>
+    <t>TERMINAR DE CODIFICAR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd\.mm\.yyyy"/>
+    <numFmt numFmtId="165" formatCode="dd\,mm\,yyyy"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -153,6 +174,17 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -202,7 +234,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -222,11 +254,36 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="24">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -240,6 +297,149 @@
         <patternFill patternType="solid">
           <fgColor rgb="FF76A5AF"/>
           <bgColor rgb="FF76A5AF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF93C47D"/>
+          <bgColor rgb="FF93C47D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF76A5AF"/>
+          <bgColor rgb="FF76A5AF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF93C47D"/>
+          <bgColor rgb="FF93C47D"/>
         </patternFill>
       </fill>
     </dxf>
@@ -522,10 +722,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:BT595"/>
+  <dimension ref="A1:FX595"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A187" workbookViewId="0">
-      <selection activeCell="B192" sqref="B192"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A104" workbookViewId="0">
+      <selection activeCell="B164" sqref="B164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -539,7 +739,7 @@
     <col min="7" max="72" width="4.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:72" ht="91.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:180" ht="91.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="8" t="s">
         <v>6</v>
@@ -615,81 +815,547 @@
       <c r="BS1" s="2"/>
       <c r="BT1" s="2"/>
     </row>
-    <row r="2" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:180" ht="61.5" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3"/>
-      <c r="Y2" s="3"/>
-      <c r="Z2" s="3"/>
-      <c r="AA2" s="3"/>
-      <c r="AB2" s="3"/>
-      <c r="AC2" s="3"/>
-      <c r="AD2" s="3"/>
-      <c r="AE2" s="3"/>
-      <c r="AF2" s="3"/>
-      <c r="AG2" s="3"/>
-      <c r="AH2" s="3"/>
-      <c r="AI2" s="3"/>
-      <c r="AJ2" s="3"/>
-      <c r="AK2" s="3"/>
-      <c r="AL2" s="3"/>
-      <c r="AM2" s="3"/>
-      <c r="AN2" s="3"/>
-      <c r="AO2" s="3"/>
-      <c r="AP2" s="3"/>
-      <c r="AQ2" s="3"/>
-      <c r="AR2" s="3"/>
-      <c r="AS2" s="3"/>
-      <c r="AT2" s="3"/>
-      <c r="AU2" s="3"/>
-      <c r="AV2" s="3"/>
-      <c r="AW2" s="3"/>
-      <c r="AX2" s="3"/>
-      <c r="AY2" s="3"/>
-      <c r="AZ2" s="3"/>
-      <c r="BA2" s="3"/>
-      <c r="BB2" s="3"/>
-      <c r="BC2" s="3"/>
-      <c r="BD2" s="3"/>
-      <c r="BE2" s="3"/>
-      <c r="BF2" s="3"/>
-      <c r="BG2" s="3"/>
-      <c r="BH2" s="3"/>
-      <c r="BI2" s="3"/>
-      <c r="BJ2" s="3"/>
-      <c r="BK2" s="3"/>
-      <c r="BL2" s="3"/>
-      <c r="BM2" s="3"/>
-      <c r="BN2" s="3"/>
-      <c r="BO2" s="3"/>
-      <c r="BP2" s="3"/>
-      <c r="BQ2" s="3"/>
-      <c r="BR2" s="3"/>
-      <c r="BS2" s="3"/>
-      <c r="BT2" s="3"/>
-    </row>
-    <row r="3" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B2" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="12">
+        <v>45418</v>
+      </c>
+      <c r="H2" s="12">
+        <v>45419</v>
+      </c>
+      <c r="I2" s="12">
+        <v>45420</v>
+      </c>
+      <c r="J2" s="12">
+        <v>45421</v>
+      </c>
+      <c r="K2" s="12">
+        <v>45422</v>
+      </c>
+      <c r="L2" s="12">
+        <v>45423</v>
+      </c>
+      <c r="M2" s="12">
+        <v>45424</v>
+      </c>
+      <c r="N2" s="12">
+        <v>45425</v>
+      </c>
+      <c r="O2" s="12">
+        <v>45426</v>
+      </c>
+      <c r="P2" s="12">
+        <v>45427</v>
+      </c>
+      <c r="Q2" s="12">
+        <v>45428</v>
+      </c>
+      <c r="R2" s="12">
+        <v>45429</v>
+      </c>
+      <c r="S2" s="12">
+        <v>45430</v>
+      </c>
+      <c r="T2" s="12">
+        <v>45431</v>
+      </c>
+      <c r="U2" s="12">
+        <v>45432</v>
+      </c>
+      <c r="V2" s="12">
+        <v>45433</v>
+      </c>
+      <c r="W2" s="12">
+        <v>45434</v>
+      </c>
+      <c r="X2" s="12">
+        <v>45435</v>
+      </c>
+      <c r="Y2" s="12">
+        <v>45436</v>
+      </c>
+      <c r="Z2" s="12">
+        <v>45437</v>
+      </c>
+      <c r="AA2" s="12">
+        <v>45438</v>
+      </c>
+      <c r="AB2" s="12">
+        <v>45439</v>
+      </c>
+      <c r="AC2" s="12">
+        <v>45440</v>
+      </c>
+      <c r="AD2" s="12">
+        <v>45441</v>
+      </c>
+      <c r="AE2" s="12">
+        <v>45442</v>
+      </c>
+      <c r="AF2" s="12">
+        <v>45443</v>
+      </c>
+      <c r="AG2" s="12">
+        <v>45444</v>
+      </c>
+      <c r="AH2" s="12">
+        <v>45445</v>
+      </c>
+      <c r="AI2" s="12">
+        <v>45446</v>
+      </c>
+      <c r="AJ2" s="12">
+        <v>45447</v>
+      </c>
+      <c r="AK2" s="12">
+        <v>45448</v>
+      </c>
+      <c r="AL2" s="12">
+        <v>45449</v>
+      </c>
+      <c r="AM2" s="12">
+        <v>45450</v>
+      </c>
+      <c r="AN2" s="12">
+        <v>45451</v>
+      </c>
+      <c r="AO2" s="12">
+        <v>45452</v>
+      </c>
+      <c r="AP2" s="12">
+        <v>45453</v>
+      </c>
+      <c r="AQ2" s="12">
+        <v>45454</v>
+      </c>
+      <c r="AR2" s="12">
+        <v>45455</v>
+      </c>
+      <c r="AS2" s="12">
+        <v>45456</v>
+      </c>
+      <c r="AT2" s="12">
+        <v>45457</v>
+      </c>
+      <c r="AU2" s="12">
+        <v>45458</v>
+      </c>
+      <c r="AV2" s="12">
+        <v>45459</v>
+      </c>
+      <c r="AW2" s="12">
+        <v>45460</v>
+      </c>
+      <c r="AX2" s="12">
+        <v>45461</v>
+      </c>
+      <c r="AY2" s="12">
+        <v>45462</v>
+      </c>
+      <c r="AZ2" s="12">
+        <v>45463</v>
+      </c>
+      <c r="BA2" s="12">
+        <v>45464</v>
+      </c>
+      <c r="BB2" s="12">
+        <v>45465</v>
+      </c>
+      <c r="BC2" s="12">
+        <v>45466</v>
+      </c>
+      <c r="BD2" s="12">
+        <v>45467</v>
+      </c>
+      <c r="BE2" s="12">
+        <v>45468</v>
+      </c>
+      <c r="BF2" s="12">
+        <v>45469</v>
+      </c>
+      <c r="BG2" s="12">
+        <v>45470</v>
+      </c>
+      <c r="BH2" s="12">
+        <v>45471</v>
+      </c>
+      <c r="BI2" s="12">
+        <v>45472</v>
+      </c>
+      <c r="BJ2" s="12">
+        <v>45473</v>
+      </c>
+      <c r="BK2" s="12">
+        <v>45474</v>
+      </c>
+      <c r="BL2" s="12">
+        <v>45475</v>
+      </c>
+      <c r="BM2" s="12">
+        <v>45476</v>
+      </c>
+      <c r="BN2" s="12">
+        <v>45477</v>
+      </c>
+      <c r="BO2" s="12">
+        <v>45478</v>
+      </c>
+      <c r="BP2" s="12">
+        <v>45479</v>
+      </c>
+      <c r="BQ2" s="12">
+        <v>45480</v>
+      </c>
+      <c r="BR2" s="12">
+        <v>45481</v>
+      </c>
+      <c r="BS2" s="12">
+        <v>45482</v>
+      </c>
+      <c r="BT2" s="12">
+        <v>45483</v>
+      </c>
+      <c r="BU2" s="12">
+        <v>45484</v>
+      </c>
+      <c r="BV2" s="12">
+        <v>45485</v>
+      </c>
+      <c r="BW2" s="12">
+        <v>45486</v>
+      </c>
+      <c r="BX2" s="12">
+        <v>45487</v>
+      </c>
+      <c r="BY2" s="12">
+        <v>45488</v>
+      </c>
+      <c r="BZ2" s="12">
+        <v>45489</v>
+      </c>
+      <c r="CA2" s="12">
+        <v>45490</v>
+      </c>
+      <c r="CB2" s="12">
+        <v>45491</v>
+      </c>
+      <c r="CC2" s="12">
+        <v>45492</v>
+      </c>
+      <c r="CD2" s="12">
+        <v>45493</v>
+      </c>
+      <c r="CE2" s="12">
+        <v>45494</v>
+      </c>
+      <c r="CF2" s="12">
+        <v>45495</v>
+      </c>
+      <c r="CG2" s="12">
+        <v>45496</v>
+      </c>
+      <c r="CH2" s="12">
+        <v>45497</v>
+      </c>
+      <c r="CI2" s="12">
+        <v>45498</v>
+      </c>
+      <c r="CJ2" s="12">
+        <v>45499</v>
+      </c>
+      <c r="CK2" s="12">
+        <v>45500</v>
+      </c>
+      <c r="CL2" s="12">
+        <v>45501</v>
+      </c>
+      <c r="CM2" s="12">
+        <v>45502</v>
+      </c>
+      <c r="CN2" s="12">
+        <v>45503</v>
+      </c>
+      <c r="CO2" s="12">
+        <v>45504</v>
+      </c>
+      <c r="CP2" s="12">
+        <v>45505</v>
+      </c>
+      <c r="CQ2" s="12">
+        <v>45506</v>
+      </c>
+      <c r="CR2" s="12">
+        <v>45507</v>
+      </c>
+      <c r="CS2" s="12">
+        <v>45508</v>
+      </c>
+      <c r="CT2" s="12">
+        <v>45509</v>
+      </c>
+      <c r="CU2" s="12">
+        <v>45510</v>
+      </c>
+      <c r="CV2" s="12">
+        <v>45511</v>
+      </c>
+      <c r="CW2" s="12">
+        <v>45512</v>
+      </c>
+      <c r="CX2" s="12">
+        <v>45513</v>
+      </c>
+      <c r="CY2" s="12">
+        <v>45514</v>
+      </c>
+      <c r="CZ2" s="12">
+        <v>45515</v>
+      </c>
+      <c r="DA2" s="12">
+        <v>45516</v>
+      </c>
+      <c r="DB2" s="12">
+        <v>45517</v>
+      </c>
+      <c r="DC2" s="12">
+        <v>45518</v>
+      </c>
+      <c r="DD2" s="12">
+        <v>45519</v>
+      </c>
+      <c r="DE2" s="12">
+        <v>45520</v>
+      </c>
+      <c r="DF2" s="12">
+        <v>45521</v>
+      </c>
+      <c r="DG2" s="12">
+        <v>45522</v>
+      </c>
+      <c r="DH2" s="12">
+        <v>45523</v>
+      </c>
+      <c r="DI2" s="12">
+        <v>45524</v>
+      </c>
+      <c r="DJ2" s="12">
+        <v>45525</v>
+      </c>
+      <c r="DK2" s="12">
+        <v>45526</v>
+      </c>
+      <c r="DL2" s="12">
+        <v>45527</v>
+      </c>
+      <c r="DM2" s="12">
+        <v>45528</v>
+      </c>
+      <c r="DN2" s="12">
+        <v>45529</v>
+      </c>
+      <c r="DO2" s="12">
+        <v>45530</v>
+      </c>
+      <c r="DP2" s="12">
+        <v>45531</v>
+      </c>
+      <c r="DQ2" s="12">
+        <v>45532</v>
+      </c>
+      <c r="DR2" s="12">
+        <v>45533</v>
+      </c>
+      <c r="DS2" s="12">
+        <v>45534</v>
+      </c>
+      <c r="DT2" s="12">
+        <v>45535</v>
+      </c>
+      <c r="DU2" s="12">
+        <v>45536</v>
+      </c>
+      <c r="DV2" s="12">
+        <v>45537</v>
+      </c>
+      <c r="DW2" s="12">
+        <v>45538</v>
+      </c>
+      <c r="DX2" s="12">
+        <v>45539</v>
+      </c>
+      <c r="DY2" s="12">
+        <v>45540</v>
+      </c>
+      <c r="DZ2" s="12">
+        <v>45541</v>
+      </c>
+      <c r="EA2" s="12">
+        <v>45542</v>
+      </c>
+      <c r="EB2" s="12">
+        <v>45543</v>
+      </c>
+      <c r="EC2" s="12">
+        <v>45544</v>
+      </c>
+      <c r="ED2" s="12">
+        <v>45545</v>
+      </c>
+      <c r="EE2" s="12">
+        <v>45546</v>
+      </c>
+      <c r="EF2" s="12">
+        <v>45547</v>
+      </c>
+      <c r="EG2" s="12">
+        <v>45548</v>
+      </c>
+      <c r="EH2" s="12">
+        <v>45549</v>
+      </c>
+      <c r="EI2" s="12">
+        <v>45550</v>
+      </c>
+      <c r="EJ2" s="12">
+        <v>45551</v>
+      </c>
+      <c r="EK2" s="12">
+        <v>45552</v>
+      </c>
+      <c r="EL2" s="12">
+        <v>45553</v>
+      </c>
+      <c r="EM2" s="12">
+        <v>45554</v>
+      </c>
+      <c r="EN2" s="12">
+        <v>45555</v>
+      </c>
+      <c r="EO2" s="12">
+        <v>45556</v>
+      </c>
+      <c r="EP2" s="12">
+        <v>45557</v>
+      </c>
+      <c r="EQ2" s="12">
+        <v>45558</v>
+      </c>
+      <c r="ER2" s="12">
+        <v>45559</v>
+      </c>
+      <c r="ES2" s="12">
+        <v>45560</v>
+      </c>
+      <c r="ET2" s="12">
+        <v>45561</v>
+      </c>
+      <c r="EU2" s="12">
+        <v>45562</v>
+      </c>
+      <c r="EV2" s="12">
+        <v>45563</v>
+      </c>
+      <c r="EW2" s="12">
+        <v>45564</v>
+      </c>
+      <c r="EX2" s="12">
+        <v>45565</v>
+      </c>
+      <c r="EY2" s="12">
+        <v>45566</v>
+      </c>
+      <c r="EZ2" s="12">
+        <v>45567</v>
+      </c>
+      <c r="FA2" s="12">
+        <v>45568</v>
+      </c>
+      <c r="FB2" s="12">
+        <v>45569</v>
+      </c>
+      <c r="FC2" s="12">
+        <v>45570</v>
+      </c>
+      <c r="FD2" s="12">
+        <v>45571</v>
+      </c>
+      <c r="FE2" s="12">
+        <v>45572</v>
+      </c>
+      <c r="FF2" s="12">
+        <v>45573</v>
+      </c>
+      <c r="FG2" s="12">
+        <v>45574</v>
+      </c>
+      <c r="FH2" s="12">
+        <v>45575</v>
+      </c>
+      <c r="FI2" s="12">
+        <v>45576</v>
+      </c>
+      <c r="FJ2" s="12">
+        <v>45577</v>
+      </c>
+      <c r="FK2" s="12">
+        <v>45578</v>
+      </c>
+      <c r="FL2" s="12">
+        <v>45579</v>
+      </c>
+      <c r="FM2" s="12">
+        <v>45580</v>
+      </c>
+      <c r="FN2" s="12">
+        <v>45581</v>
+      </c>
+      <c r="FO2" s="12">
+        <v>45582</v>
+      </c>
+      <c r="FP2" s="12">
+        <v>45583</v>
+      </c>
+      <c r="FQ2" s="12">
+        <v>45584</v>
+      </c>
+      <c r="FR2" s="12">
+        <v>45585</v>
+      </c>
+      <c r="FS2" s="12">
+        <v>45586</v>
+      </c>
+      <c r="FT2" s="12">
+        <v>45587</v>
+      </c>
+      <c r="FU2" s="12">
+        <v>45588</v>
+      </c>
+      <c r="FV2" s="12">
+        <v>45589</v>
+      </c>
+      <c r="FW2" s="12">
+        <v>45590</v>
+      </c>
+      <c r="FX2" s="12">
+        <v>45591</v>
+      </c>
+    </row>
+    <row r="3" spans="1:180" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="4" t="s">
         <v>14</v>
@@ -698,13 +1364,14 @@
         <v>45418</v>
       </c>
       <c r="D3" s="5">
-        <v>45418</v>
+        <v>45510</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="5"/>
-      <c r="G3" s="3"/>
+      <c r="F3" s="14" t="s">
+        <v>37</v>
+      </c>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
@@ -771,7 +1438,7 @@
       <c r="BS3" s="3"/>
       <c r="BT3" s="3"/>
     </row>
-    <row r="4" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:180" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5">
@@ -849,7 +1516,7 @@
       <c r="BS4" s="3"/>
       <c r="BT4" s="3"/>
     </row>
-    <row r="5" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:180" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5">
@@ -865,7 +1532,6 @@
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
@@ -927,7 +1593,7 @@
       <c r="BS5" s="3"/>
       <c r="BT5" s="3"/>
     </row>
-    <row r="6" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:180" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="4" t="s">
         <v>18</v>
@@ -1007,7 +1673,7 @@
       <c r="BS6" s="3"/>
       <c r="BT6" s="3"/>
     </row>
-    <row r="7" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:180" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5">
@@ -1085,7 +1751,7 @@
       <c r="BS7" s="3"/>
       <c r="BT7" s="3"/>
     </row>
-    <row r="8" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:180" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="4"/>
       <c r="C8" s="5">
@@ -1163,7 +1829,7 @@
       <c r="BS8" s="3"/>
       <c r="BT8" s="3"/>
     </row>
-    <row r="9" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:180" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="4"/>
       <c r="C9" s="5">
@@ -1241,7 +1907,7 @@
       <c r="BS9" s="3"/>
       <c r="BT9" s="3"/>
     </row>
-    <row r="10" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:180" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="4" t="s">
         <v>15</v>
@@ -1249,12 +1915,16 @@
       <c r="C10" s="5">
         <v>45425</v>
       </c>
-      <c r="D10" s="5"/>
+      <c r="D10" s="5">
+        <v>45425</v>
+      </c>
       <c r="E10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="5"/>
-      <c r="G10" s="3"/>
+      <c r="F10" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="G10" s="13"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
@@ -1321,7 +1991,7 @@
       <c r="BS10" s="3"/>
       <c r="BT10" s="3"/>
     </row>
-    <row r="11" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:180" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="4"/>
       <c r="C11" s="5">
@@ -1399,7 +2069,7 @@
       <c r="BS11" s="3"/>
       <c r="BT11" s="3"/>
     </row>
-    <row r="12" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:180" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="4"/>
       <c r="C12" s="5">
@@ -1477,7 +2147,7 @@
       <c r="BS12" s="3"/>
       <c r="BT12" s="3"/>
     </row>
-    <row r="13" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:180" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="4" t="s">
         <v>13</v>
@@ -1557,7 +2227,7 @@
       <c r="BS13" s="3"/>
       <c r="BT13" s="3"/>
     </row>
-    <row r="14" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:180" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="4"/>
       <c r="C14" s="5">
@@ -1635,7 +2305,7 @@
       <c r="BS14" s="3"/>
       <c r="BT14" s="3"/>
     </row>
-    <row r="15" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:180" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="4"/>
       <c r="C15" s="5">
@@ -1713,7 +2383,7 @@
       <c r="BS15" s="3"/>
       <c r="BT15" s="3"/>
     </row>
-    <row r="16" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:180" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="4"/>
       <c r="C16" s="5">
@@ -2429,7 +3099,9 @@
       <c r="E25" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F25" s="5"/>
+      <c r="F25" s="14" t="s">
+        <v>37</v>
+      </c>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
@@ -4227,7 +4899,9 @@
       <c r="C48" s="5">
         <v>45463</v>
       </c>
-      <c r="D48" s="5"/>
+      <c r="D48" s="5">
+        <v>45463</v>
+      </c>
       <c r="E48" s="5" t="s">
         <v>12</v>
       </c>
@@ -12971,8 +13645,8 @@
     </row>
     <row r="160" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A160" s="1"/>
-      <c r="B160" s="4" t="s">
-        <v>30</v>
+      <c r="B160" s="15" t="s">
+        <v>38</v>
       </c>
       <c r="C160" s="5">
         <v>45575</v>
@@ -13052,7 +13726,7 @@
     <row r="161" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A161" s="1"/>
       <c r="B161" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C161" s="5">
         <v>45576</v>
@@ -15394,7 +16068,7 @@
     <row r="191" spans="1:72" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A191" s="1"/>
       <c r="B191" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C191" s="5">
         <v>45606</v>
@@ -45554,19 +46228,97 @@
     <mergeCell ref="B1:K1"/>
     <mergeCell ref="L1:AH1"/>
   </mergeCells>
-  <conditionalFormatting sqref="G2:BT595">
-    <cfRule type="notContainsBlanks" dxfId="1" priority="1">
-      <formula>LEN(TRIM(G2))&gt;0</formula>
+  <conditionalFormatting sqref="H3:I3 G4:I4 M5:BT5 G5:K5 J3:BT4 G6:BT595">
+    <cfRule type="notContainsBlanks" dxfId="3" priority="21">
+      <formula>LEN(TRIM(G3))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:BT595">
-    <cfRule type="expression" dxfId="0" priority="4">
-      <formula>AND($C2&lt;=#REF!,$D2&gt;=#REF!)</formula>
+  <conditionalFormatting sqref="M5:BT5 G5:K5 H3:BT4 G6:BT595">
+    <cfRule type="expression" dxfId="2" priority="24">
+      <formula>AND($C3&lt;=#REF!,$D3&gt;=#REF!)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G4">
+    <cfRule type="expression" dxfId="23" priority="28">
+      <formula>AND($C3&lt;=#REF!,$D3&gt;=#REF!)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:I5 K5 J4:K4 K3 G6:K8 L6:N6">
+    <cfRule type="expression" dxfId="22" priority="17">
+      <formula>"'=Y(G$2&gt;=$C3,+G$2&lt;=$D3)"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:I3">
+    <cfRule type="expression" dxfId="21" priority="15">
+      <formula>AND(G$2&gt;=$C$3, G$2&lt;=$D$3)</formula>
+    </cfRule>
+    <cfRule type="expression" priority="16">
+      <formula>AND(G$2&gt;=$C$3, G$2&lt;=$D$3)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J6:N6">
+    <cfRule type="expression" dxfId="20" priority="13">
+      <formula>AND(J$2&gt;=$C$3, J$2&lt;=$D$3)</formula>
+    </cfRule>
+    <cfRule type="expression" priority="14">
+      <formula>AND(J$2&gt;=$C$3, J$2&lt;=$D$3)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q14">
+    <cfRule type="expression" dxfId="11" priority="12">
+      <formula>"'=Y(G$2&gt;=$C3,+G$2&lt;=$D3)"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q14">
+    <cfRule type="expression" dxfId="10" priority="10">
+      <formula>AND(Q$2&gt;=$C$3, Q$2&lt;=$D$3)</formula>
+    </cfRule>
+    <cfRule type="expression" priority="11">
+      <formula>AND(Q$2&gt;=$C$3, Q$2&lt;=$D$3)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U18:AC18">
+    <cfRule type="expression" dxfId="9" priority="9">
+      <formula>"'=Y(G$2&gt;=$C3,+G$2&lt;=$D3)"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U18:AC18">
+    <cfRule type="expression" dxfId="8" priority="7">
+      <formula>AND(U$2&gt;=$C$3, U$2&lt;=$D$3)</formula>
+    </cfRule>
+    <cfRule type="expression" priority="8">
+      <formula>AND(U$2&gt;=$C$3, U$2&lt;=$D$3)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD19:AI19">
+    <cfRule type="expression" dxfId="7" priority="6">
+      <formula>"'=Y(G$2&gt;=$C3,+G$2&lt;=$D3)"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD19:AI19">
+    <cfRule type="expression" dxfId="6" priority="4">
+      <formula>AND(AD$2&gt;=$C$3, AD$2&lt;=$D$3)</formula>
+    </cfRule>
+    <cfRule type="expression" priority="5">
+      <formula>AND(AD$2&gt;=$C$3, AD$2&lt;=$D$3)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AN36:AZ36">
+    <cfRule type="expression" dxfId="1" priority="3">
+      <formula>"'=Y(G$2&gt;=$C3,+G$2&lt;=$D3)"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AN36:AZ36">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>AND(AN$2&gt;=$C$3, AN$2&lt;=$D$3)</formula>
+    </cfRule>
+    <cfRule type="expression" priority="2">
+      <formula>AND(AN$2&gt;=$C$3, AN$2&lt;=$D$3)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="C2:F595">
-      <formula1>OR(NOT(ISERROR(DATEVALUE(C2))), AND(ISNUMBER(C2), LEFT(CELL("format", C2))="D"))</formula1>
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="C3:F595">
+      <formula1>OR(NOT(ISERROR(DATEVALUE(C3))), AND(ISNUMBER(C3), LEFT(CELL("format", C3))="D"))</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>